<commit_message>
Deploying to gh-pages from  @ 51c63f6b964405c7230bb47e8c64a0e3d95fec99 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.5.1.1.xlsx
+++ b/en/downloads/data-excel/10.5.1.1.xlsx
@@ -177,10 +177,13 @@
     <t>*according to the NBKR</t>
   </si>
   <si>
+    <t>10.5.1.1 Финансылык туруктуулуктун көрсөткүчтөрү</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <vertAlign val="superscript"/>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -190,7 +193,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -203,7 +206,7 @@
     <r>
       <rPr>
         <vertAlign val="superscript"/>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -213,7 +216,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -226,7 +229,7 @@
     <r>
       <rPr>
         <vertAlign val="superscript"/>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -236,7 +239,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -249,7 +252,7 @@
     <r>
       <rPr>
         <vertAlign val="superscript"/>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -259,7 +262,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -272,7 +275,7 @@
     <r>
       <rPr>
         <vertAlign val="superscript"/>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -282,7 +285,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -295,7 +298,7 @@
     <r>
       <rPr>
         <vertAlign val="superscript"/>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -305,7 +308,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="9"/>
+        <sz val="8"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -313,9 +316,6 @@
       </rPr>
       <t xml:space="preserve"> excluding loans granted to banks and other financial and credit organizations</t>
     </r>
-  </si>
-  <si>
-    <t>10.5.1.1 Финансылык туруктуулуктун көрсөткүчтөрү</t>
   </si>
 </sst>
 </file>
@@ -325,7 +325,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,6 +401,28 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -444,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -485,10 +507,16 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -795,24 +823,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="1" max="3" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -833,7 +857,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -858,7 +882,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="2"/>
@@ -877,7 +901,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -935,8 +959,11 @@
       <c r="S4" s="7">
         <v>2022</v>
       </c>
+      <c r="T4" s="7">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -994,8 +1021,11 @@
       <c r="S5" s="11">
         <v>49.7</v>
       </c>
+      <c r="T5" s="11">
+        <v>50</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -1053,8 +1083,11 @@
       <c r="S6" s="11">
         <v>34.9</v>
       </c>
+      <c r="T6" s="11">
+        <v>35.1</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>15</v>
       </c>
@@ -1112,15 +1145,18 @@
       <c r="S7" s="13">
         <v>21</v>
       </c>
+      <c r="T7" s="13">
+        <v>21</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2"/>
@@ -1138,15 +1174,15 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="16" t="s">
         <v>23</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1163,15 +1199,15 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="14" t="s">
+    <row r="10" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="17" t="s">
         <v>26</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>

</xml_diff>